<commit_message>
validated xml. still need to figure out how to add shapefiles
</commit_message>
<xml_diff>
--- a/data-raw/metadata_snorkel.xlsx
+++ b/data-raw/metadata_snorkel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobbie Flores\Dropbox (Cramer Fish Sciences)\NewPROJECTS\CBECAL-2014-Yuba_River_Restoration\WORKING\Data\EDI data uploads\snorkel\2014-2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/yuba_hallwood_edi/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CF5EDD-F5D9-41AB-A4A3-F76207BC6204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529561ED-7838-334D-A7B4-BE6062C89B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="834" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -26,17 +26,17 @@
     <sheet name="attribute" sheetId="9" r:id="rId11"/>
     <sheet name="code_definitions" sheetId="10" r:id="rId12"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">attribute!$A$1:$AMG$46</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="454">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -388,18 +388,6 @@
     <t>Hallwood Floodplain and Side Channel Restoration Project, Marysville, CA</t>
   </si>
   <si>
-    <t>39.189071, -121.492659</t>
-  </si>
-  <si>
-    <t>39.206902, -121.446322</t>
-  </si>
-  <si>
-    <t>39.205299, -121.455994</t>
-  </si>
-  <si>
-    <t>39.188731, -121.485588</t>
-  </si>
-  <si>
     <t>CVPIA_common_species</t>
   </si>
   <si>
@@ -529,15 +517,6 @@
     <t>dateTime</t>
   </si>
   <si>
-    <t>YYYY-MM-DDThh:mm:ss</t>
-  </si>
-  <si>
-    <t>2014-01-0100:00:00</t>
-  </si>
-  <si>
-    <t>ongoing</t>
-  </si>
-  <si>
     <t>SnorkelTransectNo</t>
   </si>
   <si>
@@ -568,9 +547,6 @@
     <t>numeric</t>
   </si>
   <si>
-    <t>meters</t>
-  </si>
-  <si>
     <t>real</t>
   </si>
   <si>
@@ -1418,12 +1394,31 @@
   </si>
   <si>
     <t>annually</t>
+  </si>
+  <si>
+    <t>CCO</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD hh:mm:ss</t>
+  </si>
+  <si>
+    <t>unique project identifier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1505,7 +1500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1551,6 +1546,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1940,16 +1941,16 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
     <col min="3" max="3" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1960,7 +1961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1968,7 +1969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1997,56 +1998,56 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.75" customWidth="1"/>
-    <col min="2" max="2" width="20.25" style="10" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="10" customWidth="1"/>
     <col min="3" max="3" width="21" style="10" customWidth="1"/>
     <col min="4" max="8" width="10.5" style="10"/>
-    <col min="9" max="9" width="10.25" style="10" customWidth="1"/>
-    <col min="10" max="10" width="32.625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="10" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>124</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2062,620 +2063,605 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG45"/>
+  <dimension ref="A1:AMG46"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.75" style="1"/>
+    <col min="1" max="2" width="19.6640625" style="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.25" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.75" style="14" customWidth="1"/>
-    <col min="6" max="6" width="5.25" style="9" customWidth="1"/>
-    <col min="7" max="7" width="5.625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="9" customWidth="1"/>
-    <col min="9" max="9" width="14.125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" style="7" customWidth="1"/>
     <col min="10" max="10" width="16" style="9" customWidth="1"/>
-    <col min="11" max="11" width="17.625" style="7" customWidth="1"/>
-    <col min="12" max="13" width="9.25" style="9" customWidth="1"/>
-    <col min="14" max="1021" width="19.75" style="1"/>
-    <col min="1022" max="1024" width="8.25" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="7" customWidth="1"/>
+    <col min="12" max="13" width="18.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="1021" width="19.6640625" style="1"/>
+    <col min="1022" max="1024" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="H1" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="I1" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="M1" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>138</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="C3" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="E3" s="14" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="J3" s="8"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="13"/>
+    </row>
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E2" s="14" t="s">
+    </row>
+    <row r="5" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>145</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="13"/>
-    </row>
-    <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B5" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>149</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>151</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>153</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="L9" s="27">
+        <v>41640</v>
+      </c>
+      <c r="M9" s="27">
+        <v>44831</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="J8" s="18" t="s">
+      <c r="E11" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="J11" s="18" t="s">
+        <v>452</v>
+      </c>
+      <c r="L11" s="28">
+        <v>41640</v>
+      </c>
+      <c r="M11" s="28">
+        <v>44831</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>160</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="B12" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="C12" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>452</v>
+      </c>
+      <c r="L12" s="28">
+        <v>41640</v>
+      </c>
+      <c r="M12" s="28">
+        <v>44831</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B13" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E13" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="F13" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>166</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="G10" s="12"/>
-      <c r="J10" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="J11" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="J12" s="17"/>
-      <c r="L12" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="M12" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>175</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>174</v>
       </c>
       <c r="J13" s="17"/>
       <c r="L13" s="9">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="M13" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="J14" s="17"/>
+      <c r="L14" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="M14" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="L16" s="9">
+        <v>5</v>
+      </c>
+      <c r="M16" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="H17" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="L17" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="M17" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="L18" s="9">
+        <v>50</v>
+      </c>
+      <c r="M18" s="9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="M19" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="L20" s="9">
+        <v>0</v>
+      </c>
+      <c r="M20" s="9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="J14" s="17"/>
-    </row>
-    <row r="15" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>179</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="L15" s="9">
-        <v>5</v>
-      </c>
-      <c r="M15" s="9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="L16" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="M16" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>186</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="L17" s="9">
-        <v>50</v>
-      </c>
-      <c r="M17" s="9">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>189</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="G18" s="9" t="s">
+      <c r="C22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>191</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="L18" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="M18" s="9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B23" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>193</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="B24" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="L19" s="9">
-        <v>0</v>
-      </c>
-      <c r="M19" s="9">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C24" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="E24" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>196</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E25" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>197</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>198</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B26" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>201</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>204</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="L24" s="9">
-        <v>1</v>
-      </c>
-      <c r="M24" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>206</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="9"/>
-    </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>208</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="9"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="13"/>
       <c r="M26" s="9"/>
     </row>
-    <row r="27" spans="1:13" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="17"/>
+      <c r="J27" s="18"/>
       <c r="K27" s="7"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
     </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="14" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
@@ -2686,19 +2672,19 @@
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
     </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -2709,19 +2695,19 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
     </row>
-    <row r="30" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -2732,117 +2718,107 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
     </row>
-    <row r="31" spans="1:13" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="7"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="13"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="9"/>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="1:13" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G32" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>174</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
       <c r="I32" s="7"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="9">
-        <v>0</v>
-      </c>
-      <c r="M32" s="9">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="J32" s="8"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="9"/>
+    </row>
+    <row r="33" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="14" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>224</v>
+        <v>164</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>186</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="I33" s="7"/>
-      <c r="J33" s="17"/>
+      <c r="J33" s="18"/>
       <c r="K33" s="7"/>
       <c r="L33" s="9">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="M33" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="14" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G34" s="21" t="s">
-        <v>224</v>
+        <v>164</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>216</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="17"/>
@@ -2854,202 +2830,211 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="1" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+        <v>165</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>166</v>
+      </c>
       <c r="I35" s="7"/>
       <c r="J35" s="17"/>
       <c r="K35" s="7"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-    </row>
-    <row r="36" spans="1:13" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L35" s="9">
+        <v>-0.2</v>
+      </c>
+      <c r="M35" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>171</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="F36" s="9"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="9" t="s">
-        <v>231</v>
-      </c>
+      <c r="H36" s="9"/>
       <c r="I36" s="7"/>
       <c r="J36" s="17"/>
       <c r="K36" s="7"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
     </row>
-    <row r="37" spans="1:13" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F37" s="9"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="9"/>
+        <v>165</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>223</v>
+      </c>
       <c r="I37" s="7"/>
-      <c r="J37" s="18"/>
+      <c r="J37" s="17"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-    </row>
-    <row r="38" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>224</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+    </row>
+    <row r="39" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>232</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="J42" s="18"/>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>234</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>240</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G41" s="21" t="s">
+      <c r="C43" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H41" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="J41" s="18"/>
-      <c r="L41" s="9">
-        <v>0</v>
-      </c>
-      <c r="M41" s="9">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>242</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="J42" s="17"/>
-      <c r="L42" s="9">
-        <v>-0.2</v>
-      </c>
-      <c r="M42" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>244</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="E43" s="14" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G43" s="21" t="s">
-        <v>224</v>
+        <v>164</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>216</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="J43" s="17"/>
       <c r="L43" s="9">
@@ -3059,64 +3044,95 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="J44" s="17"/>
+      <c r="L44" s="9">
+        <v>-0.2</v>
+      </c>
+      <c r="M44" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>238</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E45" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E44" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>248</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="J45" s="17"/>
-      <c r="L45" s="9">
+    </row>
+    <row r="46" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>240</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="J46" s="17"/>
+      <c r="L46" s="9">
         <v>-0.2</v>
       </c>
-      <c r="M45" s="9">
+      <c r="M46" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AMG46" xr:uid="{00000000-0001-0000-0800-000000000000}"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F45:F1006 F1:F43" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F46:F1007 F1:F44" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H45:H1048576 H1:H43" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H46:H1048576 H1:H44" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 C1:C1006" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7 C1:C1007" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1006" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1007" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3130,1237 +3146,1239 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="30.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>122</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="19">
         <v>125</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="19">
         <v>123</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="19">
         <v>121</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
         <v>124</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="19">
         <v>51</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
         <v>46</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="19">
         <v>47</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>48</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
         <v>50</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="19">
         <v>45</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="19">
         <v>49</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>6</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>0</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>1</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>10</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>11</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>2</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>3</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>4</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>5</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>6</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>7</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <v>8</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
         <v>9</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="C30" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B31" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="C31" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B32" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="C28" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="C32" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B33" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="C29" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="C33" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
         <v>285</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B34" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="C30" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="C34" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B35" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="C35" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B36" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="C36" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B37" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="C33" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="C37" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B38" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="C34" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="C38" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B39" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="C35" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="C39" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B40" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="C36" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="C40" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B41" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="C37" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="C41" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B42" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="C38" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="C42" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B43" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="C39" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+      <c r="C43" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B44" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="C40" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="C44" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B45" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="C41" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="C45" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B46" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="C42" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="C46" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="19" t="s">
         <v>311</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B47" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="C43" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="C47" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B48" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="C44" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="C48" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B49" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="C45" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="C49" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="19" t="s">
         <v>317</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B50" s="19" t="s">
         <v>318</v>
       </c>
-      <c r="C46" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="C50" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B51" s="19" t="s">
         <v>320</v>
       </c>
-      <c r="C47" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+      <c r="C51" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="B48" s="19" t="s">
+      <c r="B52" s="19" t="s">
         <v>322</v>
       </c>
-      <c r="C48" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+      <c r="C52" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="B49" s="19" t="s">
+      <c r="B53" s="19" t="s">
         <v>324</v>
       </c>
-      <c r="C49" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="C53" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B54" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="C50" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="C54" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B55" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="C51" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
+      <c r="C55" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B56" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="C52" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="C56" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="19" t="s">
         <v>331</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B57" s="19" t="s">
         <v>332</v>
       </c>
-      <c r="C53" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="19" t="s">
+      <c r="C57" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="19" t="s">
         <v>333</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>334</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="B55" s="19" t="s">
-        <v>336</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
-        <v>337</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>338</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
-        <v>339</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>340</v>
-      </c>
-      <c r="C57" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
-        <v>341</v>
       </c>
       <c r="B58" s="19" t="s">
         <v>101</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="19" t="s">
         <v>342</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B63" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="C59" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
+      <c r="C63" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="B64" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="C60" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="C64" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="19" t="s">
         <v>346</v>
       </c>
-      <c r="B61" s="19" t="s">
+      <c r="B65" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="C61" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+      <c r="C65" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="19" t="s">
         <v>348</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="B66" s="19" t="s">
         <v>349</v>
       </c>
-      <c r="C62" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
+      <c r="C66" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="19" t="s">
         <v>350</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B67" s="19" t="s">
         <v>351</v>
       </c>
-      <c r="C63" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+      <c r="C67" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="19" t="s">
         <v>352</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B68" s="19" t="s">
         <v>353</v>
       </c>
-      <c r="C64" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="19" t="s">
+      <c r="C68" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="19" t="s">
         <v>354</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="B69" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="C65" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="C69" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="19" t="s">
         <v>356</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B70" s="19" t="s">
         <v>357</v>
       </c>
-      <c r="C66" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
+      <c r="C70" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="B67" s="19" t="s">
+      <c r="B71" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="C67" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
+      <c r="C71" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="19" t="s">
         <v>360</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B72" s="19" t="s">
         <v>361</v>
       </c>
-      <c r="C68" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
+      <c r="C72" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="19" t="s">
         <v>362</v>
       </c>
-      <c r="B69" s="19" t="s">
+      <c r="B73" s="19" t="s">
         <v>363</v>
       </c>
-      <c r="C69" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
+      <c r="C73" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="19" t="s">
         <v>364</v>
       </c>
-      <c r="B70" s="19" t="s">
+      <c r="B74" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="C70" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="19" t="s">
+      <c r="C74" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="B71" s="19" t="s">
+      <c r="B75" s="19" t="s">
         <v>367</v>
       </c>
-      <c r="C71" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
+      <c r="C75" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="19" t="s">
         <v>368</v>
       </c>
-      <c r="B72" s="19" t="s">
+      <c r="B76" s="19" t="s">
         <v>369</v>
       </c>
-      <c r="C72" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+      <c r="C76" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="19" t="s">
         <v>370</v>
       </c>
-      <c r="B73" s="19" t="s">
+      <c r="B77" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="C73" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="19" t="s">
+      <c r="C77" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="19" t="s">
         <v>372</v>
       </c>
-      <c r="B74" s="19" t="s">
+      <c r="B78" s="19" t="s">
         <v>373</v>
       </c>
-      <c r="C74" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="19" t="s">
+      <c r="C78" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="19" t="s">
         <v>374</v>
       </c>
-      <c r="B75" s="19" t="s">
+      <c r="B79" s="19" t="s">
         <v>375</v>
       </c>
-      <c r="C75" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="19" t="s">
+      <c r="C79" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="19" t="s">
         <v>376</v>
       </c>
-      <c r="B76" s="19" t="s">
+      <c r="B80" s="19" t="s">
         <v>377</v>
       </c>
-      <c r="C76" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
+      <c r="C80" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="19" t="s">
         <v>378</v>
-      </c>
-      <c r="B77" s="19" t="s">
-        <v>379</v>
-      </c>
-      <c r="C77" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
-        <v>380</v>
-      </c>
-      <c r="B78" s="19" t="s">
-        <v>381</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
-        <v>382</v>
-      </c>
-      <c r="B79" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="C79" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
-        <v>384</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>385</v>
-      </c>
-      <c r="C80" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
-        <v>386</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>101</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>384</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="19" t="s">
+        <v>385</v>
+      </c>
+      <c r="B85" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="B82" s="19" t="s">
+      <c r="B86" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="C82" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
+      <c r="C86" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="19" t="s">
         <v>389</v>
       </c>
-      <c r="B83" s="19" t="s">
+      <c r="B87" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="C83" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="19" t="s">
+      <c r="C87" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B84" s="19" t="s">
+      <c r="B88" s="19" t="s">
         <v>392</v>
       </c>
-      <c r="C84" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="19" t="s">
+      <c r="C88" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B85" s="19" t="s">
+      <c r="B89" s="19" t="s">
         <v>394</v>
       </c>
-      <c r="C85" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="19" t="s">
+      <c r="C89" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="19" t="s">
         <v>395</v>
       </c>
-      <c r="B86" s="19" t="s">
+      <c r="B90" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="C86" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="19" t="s">
+      <c r="C90" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="19" t="s">
         <v>397</v>
       </c>
-      <c r="B87" s="19" t="s">
+      <c r="B91" s="19" t="s">
         <v>398</v>
       </c>
-      <c r="C87" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="19" t="s">
+      <c r="C91" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="19" t="s">
         <v>399</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B92" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="C88" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="19" t="s">
+      <c r="C92" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="19" t="s">
         <v>401</v>
       </c>
-      <c r="B89" s="19" t="s">
+      <c r="B93" s="19" t="s">
         <v>402</v>
       </c>
-      <c r="C89" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="19" t="s">
+      <c r="C93" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="19" t="s">
         <v>403</v>
       </c>
-      <c r="B90" s="19" t="s">
+      <c r="B94" s="19" t="s">
         <v>404</v>
       </c>
-      <c r="C90" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="19" t="s">
+      <c r="C94" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="19" t="s">
         <v>405</v>
       </c>
-      <c r="B91" s="19" t="s">
+      <c r="B95" s="19" t="s">
         <v>406</v>
       </c>
-      <c r="C91" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="19" t="s">
+      <c r="C95" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="19" t="s">
         <v>407</v>
       </c>
-      <c r="B92" s="19" t="s">
+      <c r="B96" s="19" t="s">
         <v>408</v>
       </c>
-      <c r="C92" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="19" t="s">
+      <c r="C96" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="19" t="s">
         <v>409</v>
       </c>
-      <c r="B93" s="19" t="s">
+      <c r="B97" s="19" t="s">
         <v>410</v>
       </c>
-      <c r="C93" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="19" t="s">
+      <c r="C97" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="B94" s="19" t="s">
+      <c r="B98" s="19" t="s">
         <v>412</v>
       </c>
-      <c r="C94" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="19" t="s">
+      <c r="C98" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="19" t="s">
         <v>413</v>
       </c>
-      <c r="B95" s="19" t="s">
+      <c r="B99" s="19" t="s">
         <v>414</v>
       </c>
-      <c r="C95" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="19" t="s">
+      <c r="C99" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="19" t="s">
         <v>415</v>
       </c>
-      <c r="B96" s="19" t="s">
+      <c r="B100" s="19" t="s">
         <v>416</v>
       </c>
-      <c r="C96" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="19" t="s">
+      <c r="C100" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="19" t="s">
         <v>417</v>
       </c>
-      <c r="B97" s="19" t="s">
+      <c r="B101" s="19" t="s">
         <v>418</v>
       </c>
-      <c r="C97" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="19" t="s">
+      <c r="C101" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="19" t="s">
         <v>419</v>
       </c>
-      <c r="B98" s="19" t="s">
+      <c r="B102" s="19" t="s">
         <v>420</v>
       </c>
-      <c r="C98" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="19" t="s">
+      <c r="C102" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="19" t="s">
         <v>421</v>
       </c>
-      <c r="B99" s="19" t="s">
+      <c r="B103" s="19" t="s">
         <v>422</v>
       </c>
-      <c r="C99" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="19" t="s">
+      <c r="C103" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="19" t="s">
         <v>423</v>
       </c>
-      <c r="B100" s="19" t="s">
+      <c r="B104" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="C100" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="19" t="s">
+      <c r="C104" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="19" t="s">
         <v>425</v>
       </c>
-      <c r="B101" s="19" t="s">
+      <c r="B105" s="19" t="s">
         <v>426</v>
       </c>
-      <c r="C101" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="19" t="s">
+      <c r="C105" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="19" t="s">
         <v>427</v>
       </c>
-      <c r="B102" s="19" t="s">
+      <c r="B106" s="19" t="s">
         <v>428</v>
       </c>
-      <c r="C102" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="19" t="s">
+      <c r="C106" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="19" t="s">
         <v>429</v>
       </c>
-      <c r="B103" s="19" t="s">
+      <c r="B107" s="19" t="s">
         <v>430</v>
       </c>
-      <c r="C103" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="19" t="s">
+      <c r="C107" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="19" t="s">
         <v>431</v>
       </c>
-      <c r="B104" s="19" t="s">
+      <c r="B108" s="19" t="s">
         <v>432</v>
       </c>
-      <c r="C104" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="19" t="s">
+      <c r="C108" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="19" t="s">
         <v>433</v>
       </c>
-      <c r="B105" s="19" t="s">
+      <c r="B109" s="19" t="s">
         <v>434</v>
       </c>
-      <c r="C105" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="19" t="s">
+      <c r="C109" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="19" t="s">
         <v>435</v>
       </c>
-      <c r="B106" s="19" t="s">
+      <c r="B110" s="19" t="s">
         <v>436</v>
       </c>
-      <c r="C106" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="19" t="s">
+      <c r="C110" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="19" t="s">
         <v>437</v>
       </c>
-      <c r="B107" s="19" t="s">
+      <c r="B111" s="19" t="s">
         <v>438</v>
       </c>
-      <c r="C107" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="19" t="s">
-        <v>439</v>
-      </c>
-      <c r="B108" s="19" t="s">
-        <v>440</v>
-      </c>
-      <c r="C108" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="19" t="s">
-        <v>441</v>
-      </c>
-      <c r="B109" s="19" t="s">
-        <v>442</v>
-      </c>
-      <c r="C109" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="19" t="s">
-        <v>443</v>
-      </c>
-      <c r="B110" s="19" t="s">
-        <v>444</v>
-      </c>
-      <c r="C110" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="19" t="s">
-        <v>445</v>
-      </c>
-      <c r="B111" s="19" t="s">
-        <v>446</v>
-      </c>
       <c r="C111" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="10">
         <v>0</v>
       </c>
@@ -4368,106 +4386,106 @@
         <v>101</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="10">
         <v>1</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="10">
         <v>2</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="10">
         <v>3</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="10">
         <v>4</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="10">
         <v>5</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="10">
         <v>6</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="10">
         <v>7</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="10">
         <v>8</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="10">
         <v>9</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -4481,17 +4499,17 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.75" customWidth="1"/>
-    <col min="5" max="5" width="27.25" style="24" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" style="24" customWidth="1"/>
     <col min="6" max="6" width="27" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -4511,7 +4529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -4528,7 +4546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -4539,13 +4557,13 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4562,7 +4580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4579,7 +4597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
@@ -4623,13 +4641,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.25" customWidth="1"/>
-    <col min="2" max="2" width="34.75" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -4637,7 +4655,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="115.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="115.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>36</v>
       </c>
@@ -4659,13 +4677,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.625" customWidth="1"/>
-    <col min="2" max="2" width="22.25" style="11" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -4673,7 +4691,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -4681,7 +4699,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -4689,7 +4707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -4697,7 +4715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -4705,7 +4723,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4713,7 +4731,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -4721,7 +4739,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -4729,7 +4747,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -4737,7 +4755,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -4745,7 +4763,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -4753,7 +4771,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -4761,7 +4779,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -4769,7 +4787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -4777,7 +4795,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -4785,7 +4803,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -4793,7 +4811,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -4801,7 +4819,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -4809,7 +4827,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -4817,7 +4835,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -4825,7 +4843,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -4833,7 +4851,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -4849,22 +4867,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.25" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="10" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="10"/>
-    <col min="4" max="4" width="15.125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="10" customWidth="1"/>
     <col min="5" max="5" width="26" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -4879,6 +4897,11 @@
       </c>
       <c r="E1" s="10" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -4900,16 +4923,16 @@
       <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9" style="10"/>
     <col min="3" max="3" width="9" style="5"/>
     <col min="4" max="4" width="9" style="10"/>
-    <col min="5" max="5" width="18.625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="10" customWidth="1"/>
     <col min="6" max="6" width="21.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -4929,7 +4952,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>69</v>
       </c>
@@ -4946,7 +4969,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>30</v>
       </c>
@@ -4963,7 +4986,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>19</v>
       </c>
@@ -4983,7 +5006,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>76</v>
       </c>
@@ -5000,7 +5023,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
@@ -5044,17 +5067,17 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="5"/>
-    <col min="6" max="6" width="17.25" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>81</v>
       </c>
@@ -5074,7 +5097,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
@@ -5088,7 +5111,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5099,7 +5122,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -5110,7 +5133,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -5124,7 +5147,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -5138,7 +5161,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -5164,16 +5187,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -5181,12 +5204,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -5212,20 +5235,20 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="77.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.75" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="24.125" customWidth="1"/>
-    <col min="5" max="5" width="23.75" customWidth="1"/>
-    <col min="8" max="8" width="53.625" customWidth="1"/>
+    <col min="1" max="1" width="77.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -5248,21 +5271,21 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>116</v>
+      <c r="B2" s="1">
+        <v>-121.492659</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-121.446322</v>
+      </c>
+      <c r="D2" s="1">
+        <v>39.205298999999997</v>
+      </c>
+      <c r="E2" s="1">
+        <v>39.188730999999997</v>
       </c>
       <c r="F2" s="3">
         <v>41640</v>
@@ -5271,33 +5294,33 @@
         <v>44561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="22"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding CVPIA and Cramer Fish Sciences to metadata keywords
</commit_message>
<xml_diff>
--- a/data-raw/metadata_snorkel.xlsx
+++ b/data-raw/metadata_snorkel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/yuba_hallwood_edi/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529561ED-7838-334D-A7B4-BE6062C89B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0062212A-D6C0-B543-942B-A762962E98F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="456">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -685,9 +685,6 @@
     <t>unique identifier for each individual fish or group of fish</t>
   </si>
   <si>
-    <t>ObsDepth</t>
-  </si>
-  <si>
     <t>depth at observation - usually only for salmonids</t>
   </si>
   <si>
@@ -1409,6 +1406,15 @@
   </si>
   <si>
     <t>unique project identifier</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>CVPIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cramer Fish Sciences </t>
   </si>
 </sst>
 </file>
@@ -1416,8 +1422,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1546,10 +1552,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2066,7 +2072,7 @@
   <dimension ref="A1:AMG46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2129,10 +2135,10 @@
     </row>
     <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>140</v>
@@ -2242,7 +2248,7 @@
         <v>155</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L9" s="27">
         <v>41640</v>
@@ -2281,7 +2287,7 @@
       </c>
       <c r="G11" s="12"/>
       <c r="J11" s="18" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L11" s="28">
         <v>41640</v>
@@ -2304,7 +2310,7 @@
         <v>155</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L12" s="28">
         <v>41640</v>
@@ -2417,7 +2423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>175</v>
       </c>
@@ -2766,10 +2772,10 @@
     </row>
     <row r="33" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>453</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>164</v>
@@ -2797,12 +2803,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>213</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>173</v>
@@ -2815,7 +2821,7 @@
         <v>164</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>166</v>
@@ -2832,10 +2838,10 @@
     </row>
     <row r="35" spans="1:13" s="1" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>173</v>
@@ -2848,7 +2854,7 @@
         <v>164</v>
       </c>
       <c r="G35" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>166</v>
@@ -2865,10 +2871,10 @@
     </row>
     <row r="36" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>218</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>140</v>
@@ -2888,10 +2894,10 @@
     </row>
     <row r="37" spans="1:13" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>164</v>
@@ -2904,10 +2910,10 @@
         <v>164</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="17"/>
@@ -2921,10 +2927,10 @@
     </row>
     <row r="38" spans="1:13" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>140</v>
@@ -2944,10 +2950,10 @@
     </row>
     <row r="39" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>140</v>
@@ -2958,10 +2964,10 @@
     </row>
     <row r="40" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>140</v>
@@ -2972,10 +2978,10 @@
     </row>
     <row r="41" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>140</v>
@@ -2986,10 +2992,10 @@
     </row>
     <row r="42" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>231</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>164</v>
@@ -3014,12 +3020,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>233</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>173</v>
@@ -3031,7 +3037,7 @@
         <v>164</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>166</v>
@@ -3046,10 +3052,10 @@
     </row>
     <row r="44" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>235</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>173</v>
@@ -3061,7 +3067,7 @@
         <v>164</v>
       </c>
       <c r="G44" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>166</v>
@@ -3076,10 +3082,10 @@
     </row>
     <row r="45" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>237</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>140</v>
@@ -3090,10 +3096,10 @@
     </row>
     <row r="46" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>239</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>164</v>
@@ -3105,7 +3111,7 @@
         <v>164</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>166</v>
@@ -3159,13 +3165,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>243</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3173,7 +3179,7 @@
         <v>122</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>138</v>
@@ -3184,7 +3190,7 @@
         <v>125</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>138</v>
@@ -3195,7 +3201,7 @@
         <v>123</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>138</v>
@@ -3206,7 +3212,7 @@
         <v>121</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>138</v>
@@ -3217,7 +3223,7 @@
         <v>124</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>138</v>
@@ -3228,7 +3234,7 @@
         <v>51</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>138</v>
@@ -3239,7 +3245,7 @@
         <v>46</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>138</v>
@@ -3250,7 +3256,7 @@
         <v>47</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>138</v>
@@ -3261,7 +3267,7 @@
         <v>48</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>138</v>
@@ -3272,7 +3278,7 @@
         <v>50</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>138</v>
@@ -3283,7 +3289,7 @@
         <v>45</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>138</v>
@@ -3294,7 +3300,7 @@
         <v>49</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>138</v>
@@ -3305,10 +3311,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>257</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3316,7 +3322,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>202</v>
@@ -3327,7 +3333,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>202</v>
@@ -3338,7 +3344,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>202</v>
@@ -3349,7 +3355,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>202</v>
@@ -3360,7 +3366,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>202</v>
@@ -3371,7 +3377,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>202</v>
@@ -3382,7 +3388,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>202</v>
@@ -3393,7 +3399,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>202</v>
@@ -3404,7 +3410,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>202</v>
@@ -3415,7 +3421,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>202</v>
@@ -3426,7 +3432,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>202</v>
@@ -3437,7 +3443,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>202</v>
@@ -3445,10 +3451,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>271</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>272</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>202</v>
@@ -3456,926 +3462,926 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>274</v>
-      </c>
       <c r="C28" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>276</v>
-      </c>
       <c r="C29" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>278</v>
-      </c>
       <c r="C30" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>280</v>
-      </c>
       <c r="C31" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>282</v>
-      </c>
       <c r="C32" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>284</v>
-      </c>
       <c r="C33" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>285</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>286</v>
-      </c>
       <c r="C34" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>288</v>
-      </c>
       <c r="C35" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>290</v>
-      </c>
       <c r="C36" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B37" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>292</v>
-      </c>
       <c r="C37" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>294</v>
-      </c>
       <c r="C38" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>296</v>
-      </c>
       <c r="C39" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>298</v>
-      </c>
       <c r="C40" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="B41" s="19" t="s">
-        <v>300</v>
-      </c>
       <c r="C41" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>302</v>
-      </c>
       <c r="C42" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>304</v>
-      </c>
       <c r="C43" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>306</v>
-      </c>
       <c r="C44" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>308</v>
-      </c>
       <c r="C45" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>310</v>
-      </c>
       <c r="C46" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>311</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>312</v>
-      </c>
       <c r="C47" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>314</v>
-      </c>
       <c r="C48" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>316</v>
-      </c>
       <c r="C49" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B50" s="19" t="s">
         <v>317</v>
       </c>
-      <c r="B50" s="19" t="s">
-        <v>318</v>
-      </c>
       <c r="C50" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="B51" s="19" t="s">
-        <v>320</v>
-      </c>
       <c r="C51" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>322</v>
-      </c>
       <c r="C52" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="B53" s="19" t="s">
-        <v>324</v>
-      </c>
       <c r="C53" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="B54" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="B54" s="19" t="s">
-        <v>326</v>
-      </c>
       <c r="C54" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="B55" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="B55" s="19" t="s">
-        <v>328</v>
-      </c>
       <c r="C55" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="B56" s="19" t="s">
-        <v>330</v>
-      </c>
       <c r="C56" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="B57" s="19" t="s">
         <v>331</v>
       </c>
-      <c r="B57" s="19" t="s">
-        <v>332</v>
-      </c>
       <c r="C57" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B58" s="19" t="s">
         <v>101</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="B59" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="B59" s="19" t="s">
-        <v>335</v>
-      </c>
       <c r="C59" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="B60" s="19" t="s">
         <v>336</v>
       </c>
-      <c r="B60" s="19" t="s">
-        <v>337</v>
-      </c>
       <c r="C60" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="B61" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="B61" s="19" t="s">
-        <v>339</v>
-      </c>
       <c r="C61" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="B62" s="19" t="s">
         <v>340</v>
       </c>
-      <c r="B62" s="19" t="s">
-        <v>341</v>
-      </c>
       <c r="C62" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="B63" s="19" t="s">
         <v>342</v>
       </c>
-      <c r="B63" s="19" t="s">
-        <v>343</v>
-      </c>
       <c r="C63" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="B64" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="B64" s="19" t="s">
-        <v>345</v>
-      </c>
       <c r="C64" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="B65" s="19" t="s">
         <v>346</v>
       </c>
-      <c r="B65" s="19" t="s">
-        <v>347</v>
-      </c>
       <c r="C65" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="B66" s="19" t="s">
         <v>348</v>
       </c>
-      <c r="B66" s="19" t="s">
-        <v>349</v>
-      </c>
       <c r="C66" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="B67" s="19" t="s">
         <v>350</v>
       </c>
-      <c r="B67" s="19" t="s">
-        <v>351</v>
-      </c>
       <c r="C67" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="B68" s="19" t="s">
         <v>352</v>
       </c>
-      <c r="B68" s="19" t="s">
-        <v>353</v>
-      </c>
       <c r="C68" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="B69" s="19" t="s">
         <v>354</v>
       </c>
-      <c r="B69" s="19" t="s">
-        <v>355</v>
-      </c>
       <c r="C69" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="B70" s="19" t="s">
         <v>356</v>
       </c>
-      <c r="B70" s="19" t="s">
-        <v>357</v>
-      </c>
       <c r="C70" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="B71" s="19" t="s">
         <v>358</v>
       </c>
-      <c r="B71" s="19" t="s">
-        <v>359</v>
-      </c>
       <c r="C71" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="B72" s="19" t="s">
         <v>360</v>
       </c>
-      <c r="B72" s="19" t="s">
-        <v>361</v>
-      </c>
       <c r="C72" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="B73" s="19" t="s">
         <v>362</v>
       </c>
-      <c r="B73" s="19" t="s">
-        <v>363</v>
-      </c>
       <c r="C73" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="B74" s="19" t="s">
         <v>364</v>
       </c>
-      <c r="B74" s="19" t="s">
-        <v>365</v>
-      </c>
       <c r="C74" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="B75" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="B75" s="19" t="s">
-        <v>367</v>
-      </c>
       <c r="C75" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="B76" s="19" t="s">
         <v>368</v>
       </c>
-      <c r="B76" s="19" t="s">
-        <v>369</v>
-      </c>
       <c r="C76" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="B77" s="19" t="s">
         <v>370</v>
       </c>
-      <c r="B77" s="19" t="s">
-        <v>371</v>
-      </c>
       <c r="C77" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="B78" s="19" t="s">
         <v>372</v>
       </c>
-      <c r="B78" s="19" t="s">
-        <v>373</v>
-      </c>
       <c r="C78" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="B79" s="19" t="s">
         <v>374</v>
       </c>
-      <c r="B79" s="19" t="s">
-        <v>375</v>
-      </c>
       <c r="C79" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="B80" s="19" t="s">
         <v>376</v>
       </c>
-      <c r="B80" s="19" t="s">
-        <v>377</v>
-      </c>
       <c r="C80" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>101</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="B82" s="19" t="s">
         <v>379</v>
       </c>
-      <c r="B82" s="19" t="s">
-        <v>380</v>
-      </c>
       <c r="C82" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="B83" s="19" t="s">
         <v>381</v>
       </c>
-      <c r="B83" s="19" t="s">
-        <v>382</v>
-      </c>
       <c r="C83" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="B84" s="19" t="s">
         <v>383</v>
       </c>
-      <c r="B84" s="19" t="s">
-        <v>384</v>
-      </c>
       <c r="C84" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="19" t="s">
+        <v>384</v>
+      </c>
+      <c r="B85" s="19" t="s">
         <v>385</v>
       </c>
-      <c r="B85" s="19" t="s">
-        <v>386</v>
-      </c>
       <c r="C85" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="B86" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="B86" s="19" t="s">
-        <v>388</v>
-      </c>
       <c r="C86" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="19" t="s">
+        <v>388</v>
+      </c>
+      <c r="B87" s="19" t="s">
         <v>389</v>
       </c>
-      <c r="B87" s="19" t="s">
-        <v>390</v>
-      </c>
       <c r="C87" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="B88" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B88" s="19" t="s">
-        <v>392</v>
-      </c>
       <c r="C88" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="19" t="s">
+        <v>392</v>
+      </c>
+      <c r="B89" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B89" s="19" t="s">
-        <v>394</v>
-      </c>
       <c r="C89" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="B90" s="19" t="s">
         <v>395</v>
       </c>
-      <c r="B90" s="19" t="s">
-        <v>396</v>
-      </c>
       <c r="C90" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="B91" s="19" t="s">
         <v>397</v>
       </c>
-      <c r="B91" s="19" t="s">
-        <v>398</v>
-      </c>
       <c r="C91" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="B92" s="19" t="s">
         <v>399</v>
       </c>
-      <c r="B92" s="19" t="s">
-        <v>400</v>
-      </c>
       <c r="C92" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="B93" s="19" t="s">
         <v>401</v>
       </c>
-      <c r="B93" s="19" t="s">
-        <v>402</v>
-      </c>
       <c r="C93" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="B94" s="19" t="s">
         <v>403</v>
       </c>
-      <c r="B94" s="19" t="s">
-        <v>404</v>
-      </c>
       <c r="C94" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="B95" s="19" t="s">
         <v>405</v>
       </c>
-      <c r="B95" s="19" t="s">
-        <v>406</v>
-      </c>
       <c r="C95" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="B96" s="19" t="s">
         <v>407</v>
       </c>
-      <c r="B96" s="19" t="s">
-        <v>408</v>
-      </c>
       <c r="C96" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="B97" s="19" t="s">
         <v>409</v>
       </c>
-      <c r="B97" s="19" t="s">
-        <v>410</v>
-      </c>
       <c r="C97" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="19" t="s">
+        <v>410</v>
+      </c>
+      <c r="B98" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="B98" s="19" t="s">
-        <v>412</v>
-      </c>
       <c r="C98" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="B99" s="19" t="s">
         <v>413</v>
       </c>
-      <c r="B99" s="19" t="s">
-        <v>414</v>
-      </c>
       <c r="C99" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="B100" s="19" t="s">
         <v>415</v>
       </c>
-      <c r="B100" s="19" t="s">
-        <v>416</v>
-      </c>
       <c r="C100" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="B101" s="19" t="s">
         <v>417</v>
       </c>
-      <c r="B101" s="19" t="s">
-        <v>418</v>
-      </c>
       <c r="C101" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="B102" s="19" t="s">
         <v>419</v>
       </c>
-      <c r="B102" s="19" t="s">
-        <v>420</v>
-      </c>
       <c r="C102" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="19" t="s">
+        <v>420</v>
+      </c>
+      <c r="B103" s="19" t="s">
         <v>421</v>
       </c>
-      <c r="B103" s="19" t="s">
-        <v>422</v>
-      </c>
       <c r="C103" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="B104" s="19" t="s">
         <v>423</v>
       </c>
-      <c r="B104" s="19" t="s">
-        <v>424</v>
-      </c>
       <c r="C104" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="s">
+        <v>424</v>
+      </c>
+      <c r="B105" s="19" t="s">
         <v>425</v>
       </c>
-      <c r="B105" s="19" t="s">
-        <v>426</v>
-      </c>
       <c r="C105" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="19" t="s">
+        <v>426</v>
+      </c>
+      <c r="B106" s="19" t="s">
         <v>427</v>
       </c>
-      <c r="B106" s="19" t="s">
-        <v>428</v>
-      </c>
       <c r="C106" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="B107" s="19" t="s">
         <v>429</v>
       </c>
-      <c r="B107" s="19" t="s">
-        <v>430</v>
-      </c>
       <c r="C107" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="19" t="s">
+        <v>430</v>
+      </c>
+      <c r="B108" s="19" t="s">
         <v>431</v>
       </c>
-      <c r="B108" s="19" t="s">
-        <v>432</v>
-      </c>
       <c r="C108" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="19" t="s">
+        <v>432</v>
+      </c>
+      <c r="B109" s="19" t="s">
         <v>433</v>
       </c>
-      <c r="B109" s="19" t="s">
-        <v>434</v>
-      </c>
       <c r="C109" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="19" t="s">
+        <v>434</v>
+      </c>
+      <c r="B110" s="19" t="s">
         <v>435</v>
       </c>
-      <c r="B110" s="19" t="s">
-        <v>436</v>
-      </c>
       <c r="C110" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="19" t="s">
+        <v>436</v>
+      </c>
+      <c r="B111" s="19" t="s">
         <v>437</v>
       </c>
-      <c r="B111" s="19" t="s">
-        <v>438</v>
-      </c>
       <c r="C111" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -4386,7 +4392,7 @@
         <v>101</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -4394,10 +4400,10 @@
         <v>1</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -4405,10 +4411,10 @@
         <v>2</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -4416,10 +4422,10 @@
         <v>3</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -4427,10 +4433,10 @@
         <v>4</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -4438,10 +4444,10 @@
         <v>5</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4449,10 +4455,10 @@
         <v>6</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4460,10 +4466,10 @@
         <v>7</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4471,10 +4477,10 @@
         <v>8</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4482,10 +4488,10 @@
         <v>9</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -4671,10 +4677,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4857,6 +4863,16 @@
       </c>
       <c r="B22" s="11" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -4901,7 +4917,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -5209,7 +5225,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating title of metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata_snorkel.xlsx
+++ b/data-raw/metadata_snorkel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/yuba_hallwood_edi/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0062212A-D6C0-B543-942B-A762962E98F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDC3F89-5005-DE49-A863-85A35E2ED025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -157,9 +157,6 @@
     <t>short_name</t>
   </si>
   <si>
-    <t>Pre- and Post- construction snorkel surveys at the project and reach stretches, 2014, 2016, 2020, 2021</t>
-  </si>
-  <si>
     <t>snorkel surveys 2014 - 2021</t>
   </si>
   <si>
@@ -1415,6 +1412,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cramer Fish Sciences </t>
+  </si>
+  <si>
+    <t>Lower Yuba River Hallwood floodplain and side channel restoration snorkel surveys at the project and control reaches</t>
   </si>
 </sst>
 </file>
@@ -1947,7 +1947,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2016,44 +2016,44 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2071,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMG46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2094,71 +2094,71 @@
   <sheetData>
     <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>141</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="6"/>
@@ -2166,89 +2166,89 @@
     </row>
     <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="E9" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L9" s="27">
         <v>41640</v>
@@ -2259,35 +2259,35 @@
     </row>
     <row r="10" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G11" s="12"/>
       <c r="J11" s="18" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L11" s="28">
         <v>41640</v>
@@ -2298,19 +2298,19 @@
     </row>
     <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L12" s="28">
         <v>41640</v>
@@ -2321,25 +2321,25 @@
     </row>
     <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="F13" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="J13" s="17"/>
       <c r="L13" s="9">
@@ -2351,25 +2351,25 @@
     </row>
     <row r="14" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="C14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="F14" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="J14" s="17"/>
       <c r="L14" s="9">
@@ -2381,40 +2381,40 @@
     </row>
     <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="E16" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="H16" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="L16" s="9">
         <v>5</v>
@@ -2425,25 +2425,25 @@
     </row>
     <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E17" s="14" t="s">
+      <c r="H17" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="L17" s="9">
         <v>1.5</v>
@@ -2454,25 +2454,25 @@
     </row>
     <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E18" s="14" t="s">
+      <c r="H18" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="L18" s="9">
         <v>50</v>
@@ -2483,25 +2483,25 @@
     </row>
     <row r="19" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E19" s="14" t="s">
+      <c r="H19" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="L19" s="9">
         <v>0.01</v>
@@ -2512,25 +2512,25 @@
     </row>
     <row r="20" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E20" s="14" t="s">
+      <c r="H20" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="L20" s="9">
         <v>0</v>
@@ -2541,87 +2541,87 @@
     </row>
     <row r="21" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="E24" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="C25" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -2634,17 +2634,17 @@
     </row>
     <row r="27" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>199</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
@@ -2657,17 +2657,17 @@
     </row>
     <row r="28" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
@@ -2680,17 +2680,17 @@
     </row>
     <row r="29" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -2703,17 +2703,17 @@
     </row>
     <row r="30" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>205</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -2726,17 +2726,17 @@
     </row>
     <row r="31" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -2749,17 +2749,17 @@
     </row>
     <row r="32" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>209</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -2772,26 +2772,26 @@
     </row>
     <row r="33" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="H33" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G33" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="18"/>
@@ -2805,26 +2805,26 @@
     </row>
     <row r="34" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>212</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="H34" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="17"/>
@@ -2838,26 +2838,26 @@
     </row>
     <row r="35" spans="1:13" s="1" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>215</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="H35" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G35" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="17"/>
@@ -2871,17 +2871,17 @@
     </row>
     <row r="36" spans="1:13" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>217</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -2894,26 +2894,26 @@
     </row>
     <row r="37" spans="1:13" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>219</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="17"/>
@@ -2927,17 +2927,17 @@
     </row>
     <row r="38" spans="1:13" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="C38" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="12"/>
@@ -2950,67 +2950,67 @@
     </row>
     <row r="39" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>230</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>232</v>
-      </c>
       <c r="C42" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="F42" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="H42" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="J42" s="18"/>
       <c r="L42" s="9">
@@ -3022,25 +3022,25 @@
     </row>
     <row r="43" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>232</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="C43" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E43" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="H43" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="J43" s="17"/>
       <c r="L43" s="9">
@@ -3052,25 +3052,25 @@
     </row>
     <row r="44" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>234</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>236</v>
-      </c>
       <c r="C44" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E44" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="H44" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G44" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="J44" s="17"/>
       <c r="L44" s="9">
@@ -3082,39 +3082,39 @@
     </row>
     <row r="45" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>236</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>238</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="C46" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E46" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="F46" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="H46" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G46" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="J46" s="17"/>
       <c r="L46" s="9">
@@ -3165,13 +3165,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>242</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3179,10 +3179,10 @@
         <v>122</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3190,10 +3190,10 @@
         <v>125</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3201,10 +3201,10 @@
         <v>123</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3212,10 +3212,10 @@
         <v>121</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3223,10 +3223,10 @@
         <v>124</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3234,10 +3234,10 @@
         <v>51</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3245,10 +3245,10 @@
         <v>46</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3256,10 +3256,10 @@
         <v>47</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -3267,10 +3267,10 @@
         <v>48</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3278,10 +3278,10 @@
         <v>50</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3289,10 +3289,10 @@
         <v>45</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3300,10 +3300,10 @@
         <v>49</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3311,10 +3311,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3322,10 +3322,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3333,10 +3333,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3344,10 +3344,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3355,10 +3355,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3366,10 +3366,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3377,10 +3377,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3388,10 +3388,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3399,10 +3399,10 @@
         <v>5</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3410,10 +3410,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3421,10 +3421,10 @@
         <v>7</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3432,10 +3432,10 @@
         <v>8</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3443,945 +3443,945 @@
         <v>9</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>271</v>
-      </c>
       <c r="C27" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>273</v>
-      </c>
       <c r="C28" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>275</v>
-      </c>
       <c r="C29" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>277</v>
-      </c>
       <c r="C30" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>279</v>
-      </c>
       <c r="C31" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>281</v>
-      </c>
       <c r="C32" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>283</v>
-      </c>
       <c r="C33" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>285</v>
-      </c>
       <c r="C34" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>287</v>
-      </c>
       <c r="C35" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>289</v>
-      </c>
       <c r="C36" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="B37" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>291</v>
-      </c>
       <c r="C37" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>293</v>
-      </c>
       <c r="C38" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>295</v>
-      </c>
       <c r="C39" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>297</v>
-      </c>
       <c r="C40" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="B41" s="19" t="s">
-        <v>299</v>
-      </c>
       <c r="C41" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>301</v>
-      </c>
       <c r="C42" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>303</v>
-      </c>
       <c r="C43" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>305</v>
-      </c>
       <c r="C44" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>307</v>
-      </c>
       <c r="C45" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="B46" s="19" t="s">
-        <v>309</v>
-      </c>
       <c r="C46" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>311</v>
-      </c>
       <c r="C47" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>313</v>
-      </c>
       <c r="C48" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>315</v>
-      </c>
       <c r="C49" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="B50" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="B50" s="19" t="s">
-        <v>317</v>
-      </c>
       <c r="C50" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>318</v>
       </c>
-      <c r="B51" s="19" t="s">
-        <v>319</v>
-      </c>
       <c r="C51" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>320</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>321</v>
-      </c>
       <c r="C52" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>322</v>
       </c>
-      <c r="B53" s="19" t="s">
-        <v>323</v>
-      </c>
       <c r="C53" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="B54" s="19" t="s">
         <v>324</v>
       </c>
-      <c r="B54" s="19" t="s">
-        <v>325</v>
-      </c>
       <c r="C54" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="B55" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="B55" s="19" t="s">
-        <v>327</v>
-      </c>
       <c r="C55" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="B56" s="19" t="s">
-        <v>329</v>
-      </c>
       <c r="C56" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="B57" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="B57" s="19" t="s">
-        <v>331</v>
-      </c>
       <c r="C57" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="B59" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="B59" s="19" t="s">
-        <v>334</v>
-      </c>
       <c r="C59" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="B60" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="B60" s="19" t="s">
-        <v>336</v>
-      </c>
       <c r="C60" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="B61" s="19" t="s">
         <v>337</v>
       </c>
-      <c r="B61" s="19" t="s">
-        <v>338</v>
-      </c>
       <c r="C61" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="B62" s="19" t="s">
         <v>339</v>
       </c>
-      <c r="B62" s="19" t="s">
-        <v>340</v>
-      </c>
       <c r="C62" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="B63" s="19" t="s">
         <v>341</v>
       </c>
-      <c r="B63" s="19" t="s">
-        <v>342</v>
-      </c>
       <c r="C63" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B64" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="B64" s="19" t="s">
-        <v>344</v>
-      </c>
       <c r="C64" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="B65" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="B65" s="19" t="s">
-        <v>346</v>
-      </c>
       <c r="C65" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="B66" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="B66" s="19" t="s">
-        <v>348</v>
-      </c>
       <c r="C66" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="B67" s="19" t="s">
         <v>349</v>
       </c>
-      <c r="B67" s="19" t="s">
-        <v>350</v>
-      </c>
       <c r="C67" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="B68" s="19" t="s">
         <v>351</v>
       </c>
-      <c r="B68" s="19" t="s">
-        <v>352</v>
-      </c>
       <c r="C68" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="B69" s="19" t="s">
         <v>353</v>
       </c>
-      <c r="B69" s="19" t="s">
-        <v>354</v>
-      </c>
       <c r="C69" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B70" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="B70" s="19" t="s">
-        <v>356</v>
-      </c>
       <c r="C70" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="B71" s="19" t="s">
         <v>357</v>
       </c>
-      <c r="B71" s="19" t="s">
-        <v>358</v>
-      </c>
       <c r="C71" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="B72" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="B72" s="19" t="s">
-        <v>360</v>
-      </c>
       <c r="C72" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
+        <v>360</v>
+      </c>
+      <c r="B73" s="19" t="s">
         <v>361</v>
       </c>
-      <c r="B73" s="19" t="s">
-        <v>362</v>
-      </c>
       <c r="C73" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="B74" s="19" t="s">
         <v>363</v>
       </c>
-      <c r="B74" s="19" t="s">
-        <v>364</v>
-      </c>
       <c r="C74" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="B75" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="B75" s="19" t="s">
-        <v>366</v>
-      </c>
       <c r="C75" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="B76" s="19" t="s">
         <v>367</v>
       </c>
-      <c r="B76" s="19" t="s">
-        <v>368</v>
-      </c>
       <c r="C76" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="B77" s="19" t="s">
         <v>369</v>
       </c>
-      <c r="B77" s="19" t="s">
-        <v>370</v>
-      </c>
       <c r="C77" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="B78" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="B78" s="19" t="s">
-        <v>372</v>
-      </c>
       <c r="C78" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="B79" s="19" t="s">
         <v>373</v>
       </c>
-      <c r="B79" s="19" t="s">
-        <v>374</v>
-      </c>
       <c r="C79" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="B80" s="19" t="s">
         <v>375</v>
       </c>
-      <c r="B80" s="19" t="s">
-        <v>376</v>
-      </c>
       <c r="C80" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="B82" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="B82" s="19" t="s">
-        <v>379</v>
-      </c>
       <c r="C82" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="B83" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="B83" s="19" t="s">
-        <v>381</v>
-      </c>
       <c r="C83" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="B84" s="19" t="s">
         <v>382</v>
       </c>
-      <c r="B84" s="19" t="s">
-        <v>383</v>
-      </c>
       <c r="C84" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="B85" s="19" t="s">
         <v>384</v>
       </c>
-      <c r="B85" s="19" t="s">
-        <v>385</v>
-      </c>
       <c r="C85" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="19" t="s">
+        <v>385</v>
+      </c>
+      <c r="B86" s="19" t="s">
         <v>386</v>
       </c>
-      <c r="B86" s="19" t="s">
-        <v>387</v>
-      </c>
       <c r="C86" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="19" t="s">
+        <v>387</v>
+      </c>
+      <c r="B87" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="B87" s="19" t="s">
-        <v>389</v>
-      </c>
       <c r="C87" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="19" t="s">
+        <v>389</v>
+      </c>
+      <c r="B88" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B88" s="19" t="s">
-        <v>391</v>
-      </c>
       <c r="C88" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="B89" s="19" t="s">
         <v>392</v>
       </c>
-      <c r="B89" s="19" t="s">
-        <v>393</v>
-      </c>
       <c r="C89" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="B90" s="19" t="s">
         <v>394</v>
       </c>
-      <c r="B90" s="19" t="s">
-        <v>395</v>
-      </c>
       <c r="C90" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="B91" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B91" s="19" t="s">
-        <v>397</v>
-      </c>
       <c r="C91" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="B92" s="19" t="s">
         <v>398</v>
       </c>
-      <c r="B92" s="19" t="s">
-        <v>399</v>
-      </c>
       <c r="C92" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="B93" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B93" s="19" t="s">
-        <v>401</v>
-      </c>
       <c r="C93" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B94" s="19" t="s">
         <v>402</v>
       </c>
-      <c r="B94" s="19" t="s">
-        <v>403</v>
-      </c>
       <c r="C94" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="B95" s="19" t="s">
         <v>404</v>
       </c>
-      <c r="B95" s="19" t="s">
-        <v>405</v>
-      </c>
       <c r="C95" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="B96" s="19" t="s">
         <v>406</v>
       </c>
-      <c r="B96" s="19" t="s">
-        <v>407</v>
-      </c>
       <c r="C96" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="B97" s="19" t="s">
         <v>408</v>
       </c>
-      <c r="B97" s="19" t="s">
-        <v>409</v>
-      </c>
       <c r="C97" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="B98" s="19" t="s">
         <v>410</v>
       </c>
-      <c r="B98" s="19" t="s">
-        <v>411</v>
-      </c>
       <c r="C98" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="B99" s="19" t="s">
         <v>412</v>
       </c>
-      <c r="B99" s="19" t="s">
-        <v>413</v>
-      </c>
       <c r="C99" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="19" t="s">
+        <v>413</v>
+      </c>
+      <c r="B100" s="19" t="s">
         <v>414</v>
       </c>
-      <c r="B100" s="19" t="s">
-        <v>415</v>
-      </c>
       <c r="C100" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="B101" s="19" t="s">
         <v>416</v>
       </c>
-      <c r="B101" s="19" t="s">
-        <v>417</v>
-      </c>
       <c r="C101" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="B102" s="19" t="s">
         <v>418</v>
       </c>
-      <c r="B102" s="19" t="s">
-        <v>419</v>
-      </c>
       <c r="C102" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="19" t="s">
+        <v>419</v>
+      </c>
+      <c r="B103" s="19" t="s">
         <v>420</v>
       </c>
-      <c r="B103" s="19" t="s">
-        <v>421</v>
-      </c>
       <c r="C103" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="s">
+        <v>421</v>
+      </c>
+      <c r="B104" s="19" t="s">
         <v>422</v>
       </c>
-      <c r="B104" s="19" t="s">
-        <v>423</v>
-      </c>
       <c r="C104" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="B105" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="B105" s="19" t="s">
-        <v>425</v>
-      </c>
       <c r="C105" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="19" t="s">
+        <v>425</v>
+      </c>
+      <c r="B106" s="19" t="s">
         <v>426</v>
       </c>
-      <c r="B106" s="19" t="s">
-        <v>427</v>
-      </c>
       <c r="C106" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="19" t="s">
+        <v>427</v>
+      </c>
+      <c r="B107" s="19" t="s">
         <v>428</v>
       </c>
-      <c r="B107" s="19" t="s">
-        <v>429</v>
-      </c>
       <c r="C107" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="B108" s="19" t="s">
         <v>430</v>
       </c>
-      <c r="B108" s="19" t="s">
-        <v>431</v>
-      </c>
       <c r="C108" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="B109" s="19" t="s">
         <v>432</v>
       </c>
-      <c r="B109" s="19" t="s">
-        <v>433</v>
-      </c>
       <c r="C109" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="19" t="s">
+        <v>433</v>
+      </c>
+      <c r="B110" s="19" t="s">
         <v>434</v>
       </c>
-      <c r="B110" s="19" t="s">
-        <v>435</v>
-      </c>
       <c r="C110" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="B111" s="19" t="s">
         <v>436</v>
       </c>
-      <c r="B111" s="19" t="s">
-        <v>437</v>
-      </c>
       <c r="C111" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -4389,10 +4389,10 @@
         <v>0</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -4400,10 +4400,10 @@
         <v>1</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -4411,10 +4411,10 @@
         <v>2</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -4422,10 +4422,10 @@
         <v>3</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -4433,10 +4433,10 @@
         <v>4</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -4444,10 +4444,10 @@
         <v>5</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -4455,10 +4455,10 @@
         <v>6</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -4466,10 +4466,10 @@
         <v>7</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -4477,10 +4477,10 @@
         <v>8</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -4488,10 +4488,10 @@
         <v>9</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -4643,8 +4643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4663,10 +4663,10 @@
     </row>
     <row r="2" spans="1:2" ht="115.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
+        <v>455</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -4691,188 +4691,188 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4900,24 +4900,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -4962,7 +4962,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>12</v>
@@ -4970,19 +4970,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>71</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5010,30 +5010,30 @@
         <v>18</v>
       </c>
       <c r="C4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>79</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>17</v>
@@ -5050,7 +5050,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>17</v>
@@ -5095,97 +5095,97 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="23" t="s">
         <v>94</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="23" t="s">
         <v>98</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>101</v>
-      </c>
       <c r="D7" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -5214,18 +5214,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -5266,30 +5266,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>110</v>
-      </c>
-      <c r="G1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1">
         <v>-121.492659</v>

</xml_diff>

<commit_message>
made requested updates to metadata and datetime formatting. passes validation and successfully uploaded to staging.
</commit_message>
<xml_diff>
--- a/data-raw/metadata_snorkel.xlsx
+++ b/data-raw/metadata_snorkel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/yuba_hallwood_edi/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDC3F89-5005-DE49-A863-85A35E2ED025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B042CD4-3636-AF46-A648-5EEB442197CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="460">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -1399,9 +1399,6 @@
     <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss</t>
-  </si>
-  <si>
     <t>unique project identifier</t>
   </si>
   <si>
@@ -1415,6 +1412,21 @@
   </si>
   <si>
     <t>Lower Yuba River Hallwood floodplain and side channel restoration snorkel surveys at the project and control reaches</t>
+  </si>
+  <si>
+    <t>DD/MM/YYYY hh:mm</t>
+  </si>
+  <si>
+    <t>6/9/2022 9:25</t>
+  </si>
+  <si>
+    <t>6/9/2022 9:36</t>
+  </si>
+  <si>
+    <t>11/12/2021 11:22</t>
+  </si>
+  <si>
+    <t>11/12/2021 11:34</t>
   </si>
 </sst>
 </file>
@@ -2071,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMG46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2138,7 +2150,7 @@
         <v>256</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>139</v>
@@ -2287,13 +2299,13 @@
       </c>
       <c r="G11" s="12"/>
       <c r="J11" s="18" t="s">
-        <v>450</v>
-      </c>
-      <c r="L11" s="28">
-        <v>41640</v>
-      </c>
-      <c r="M11" s="28">
-        <v>44831</v>
+        <v>455</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -2310,13 +2322,13 @@
         <v>154</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>450</v>
-      </c>
-      <c r="L12" s="28">
-        <v>41640</v>
-      </c>
-      <c r="M12" s="28">
-        <v>44831</v>
+        <v>455</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -2772,7 +2784,7 @@
     </row>
     <row r="33" spans="1:13" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>211</v>
@@ -4643,7 +4655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4663,7 +4675,7 @@
     </row>
     <row r="2" spans="1:2" ht="115.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -4867,12 +4879,12 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated snorkel data to fix datetime issue. values are also now characters
</commit_message>
<xml_diff>
--- a/data-raw/metadata_snorkel.xlsx
+++ b/data-raw/metadata_snorkel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/yuba_hallwood_edi/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B042CD4-3636-AF46-A648-5EEB442197CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00956E0-3638-C94C-B26C-49764069B38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="459">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -1414,30 +1414,26 @@
     <t>Lower Yuba River Hallwood floodplain and side channel restoration snorkel surveys at the project and control reaches</t>
   </si>
   <si>
-    <t>DD/MM/YYYY hh:mm</t>
-  </si>
-  <si>
-    <t>6/9/2022 9:25</t>
-  </si>
-  <si>
-    <t>6/9/2022 9:36</t>
-  </si>
-  <si>
-    <t>11/12/2021 11:22</t>
-  </si>
-  <si>
-    <t>11/12/2021 11:34</t>
+    <t>YYYY-MM-DD hh:mm:ss</t>
+  </si>
+  <si>
+    <t>2014-05-09 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-06-23 11:40:00</t>
+  </si>
+  <si>
+    <t>2022-06-23 11:52:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1477,6 +1473,12 @@
       <color rgb="FF494A4C"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1567,7 +1569,7 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2083,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMG46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2301,8 +2303,8 @@
       <c r="J11" s="18" t="s">
         <v>455</v>
       </c>
-      <c r="L11" s="9" t="s">
-        <v>458</v>
+      <c r="L11" s="28" t="s">
+        <v>456</v>
       </c>
       <c r="M11" s="28" t="s">
         <v>456</v>
@@ -2325,10 +2327,10 @@
         <v>455</v>
       </c>
       <c r="L12" s="28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M12" s="28" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -3138,6 +3140,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AMG46" xr:uid="{00000000-0001-0000-0800-000000000000}"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F46:F1007 F1:F44" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>

</xml_diff>

<commit_message>
updating time formating in data and metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata_snorkel.xlsx
+++ b/data-raw/metadata_snorkel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/yuba_hallwood_edi/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00956E0-3638-C94C-B26C-49764069B38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAFE0CE-B148-C349-B964-006B3AD5EB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1414,16 +1414,16 @@
     <t>Lower Yuba River Hallwood floodplain and side channel restoration snorkel surveys at the project and control reaches</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss</t>
-  </si>
-  <si>
-    <t>2014-05-09 00:00:00</t>
-  </si>
-  <si>
-    <t>2022-06-23 11:40:00</t>
-  </si>
-  <si>
-    <t>2022-06-23 11:52:00</t>
+    <t>hh:mm:ss</t>
+  </si>
+  <si>
+    <t> 00:00:00</t>
+  </si>
+  <si>
+    <t>16:33:00</t>
+  </si>
+  <si>
+    <t>16:34:00</t>
   </si>
 </sst>
 </file>
@@ -2086,7 +2086,7 @@
   <dimension ref="A1:AMG46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2307,7 +2307,7 @@
         <v>456</v>
       </c>
       <c r="M11" s="28" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
@@ -2327,7 +2327,7 @@
         <v>455</v>
       </c>
       <c r="L12" s="28" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="M12" s="28" t="s">
         <v>458</v>

</xml_diff>